<commit_message>
New test case added also added utils
</commit_message>
<xml_diff>
--- a/InputFile.xlsx
+++ b/InputFile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Username</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">ksgokul01@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goku!12</t>
   </si>
 </sst>
 </file>
@@ -139,7 +142,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -169,7 +172,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>